<commit_message>
is the deed done did
</commit_message>
<xml_diff>
--- a/graphics/tables.xlsx
+++ b/graphics/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29180" yWindow="1200" windowWidth="24800" windowHeight="17320" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios" sheetId="2" r:id="rId1"/>
@@ -383,15 +383,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,6 +400,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,49 +743,48 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="22" customWidth="1"/>
-    <col min="2" max="3" width="16.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="19" customWidth="1"/>
+    <col min="2" max="3" width="24.28515625" style="15" customWidth="1"/>
     <col min="4" max="16384" width="10.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="85" customHeight="1">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:3" ht="113" customHeight="1">
+      <c r="A2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="85" customHeight="1" thickBot="1">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:3" ht="113" customHeight="1" thickBot="1">
+      <c r="A3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -887,7 +886,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>